<commit_message>
DoInventory + init JavaDoc
- added doInventory
- started with JavaDoc
</commit_message>
<xml_diff>
--- a/src/main/java/ch/juventus/se/kiosk/inventoryList.xlsx
+++ b/src/main/java/ch/juventus/se/kiosk/inventoryList.xlsx
@@ -12,18 +12,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>Anzahl</t>
+    <t>Title</t>
   </si>
   <si>
-    <t>Beschreibung</t>
+    <t>Single Price</t>
   </si>
   <si>
-    <t>RedBull: CHF 3.5 (Softdrink volume in dl 2.5)</t>
+    <t>Quantity</t>
   </si>
   <si>
-    <t>Zweifel Chips: CHF 6.7 (Snack type SALTY)</t>
+    <t>Total Price</t>
+  </si>
+  <si>
+    <t>RedBull</t>
+  </si>
+  <si>
+    <t>CHF 3.5</t>
+  </si>
+  <si>
+    <t>Zweifel Chips</t>
+  </si>
+  <si>
+    <t>CHF 6.7</t>
+  </si>
+  <si>
+    <t>GRAND TOTAL:</t>
   </si>
 </sst>
 </file>
@@ -75,27 +90,53 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="n">
         <v>1.0</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
+      <c r="E2" t="n">
+        <v>3.5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2.0</v>
+      <c r="B3" t="s">
+        <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="n">
+        <v>10.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed FileHandler + UC Output
- fixed fileHandler
- fixed Formatting
- added UC Ouput files
</commit_message>
<xml_diff>
--- a/src/main/java/ch/juventus/se/kiosk/inventoryList.xlsx
+++ b/src/main/java/ch/juventus/se/kiosk/inventoryList.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Title</t>
   </si>
@@ -26,16 +26,58 @@
     <t>Total Price</t>
   </si>
   <si>
+    <t>NZZ</t>
+  </si>
+  <si>
+    <t>CHF 3.2</t>
+  </si>
+  <si>
+    <t>Salami</t>
+  </si>
+  <si>
+    <t>CHF 5.8</t>
+  </si>
+  <si>
+    <t>Vodka 0.7L</t>
+  </si>
+  <si>
+    <t>CHF 20.0</t>
+  </si>
+  <si>
+    <t>Apfel</t>
+  </si>
+  <si>
+    <t>CHF 1.0</t>
+  </si>
+  <si>
+    <t>Zweifel Paprika</t>
+  </si>
+  <si>
+    <t>CHF 6.7</t>
+  </si>
+  <si>
+    <t>Zimt Kaugummi</t>
+  </si>
+  <si>
+    <t>CHF 1.5</t>
+  </si>
+  <si>
     <t>RedBull</t>
   </si>
   <si>
     <t>CHF 3.5</t>
   </si>
   <si>
-    <t>Zweifel Chips</t>
-  </si>
-  <si>
-    <t>CHF 6.7</t>
+    <t>Quöllfrisch 0.5L</t>
+  </si>
+  <si>
+    <t>CHF 1.7</t>
+  </si>
+  <si>
+    <t>Winston BLUE</t>
+  </si>
+  <si>
+    <t>CHF 8.1</t>
   </si>
   <si>
     <t>GRAND TOTAL:</t>
@@ -111,10 +153,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.0</v>
+        <v>15.0</v>
       </c>
       <c r="D2" t="n">
-        <v>3.5</v>
+        <v>48.0</v>
       </c>
     </row>
     <row r="3">
@@ -125,18 +167,116 @@
         <v>7</v>
       </c>
       <c r="C3" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="D3" t="n">
-        <v>6.7</v>
+        <v>29.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>10.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="n">
+        <v>10.0</v>
       </c>
       <c r="D6" t="n">
-        <v>10.2</v>
+        <v>67.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>30.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>121.5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="n">
+        <v>475.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>